<commit_message>
Update Milestones - timesStandard-prod-Nov24.xlsx
</commit_message>
<xml_diff>
--- a/data/Milestones - timesStandard-prod-Nov24.xlsx
+++ b/data/Milestones - timesStandard-prod-Nov24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabiomar/Documents/GitHub/MilestonesExperiments/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A0C69219-6A08-3A46-9AF3-9CF0749BA363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D50C2E6C-53A7-454B-88B3-D396264FA295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31240" yWindow="2200" windowWidth="44800" windowHeight="16440" xr2:uid="{8DED5328-2C56-4E4D-9A47-69E3D39ABCF6}"/>
+    <workbookView xWindow="31360" yWindow="500" windowWidth="44800" windowHeight="16440" xr2:uid="{8DED5328-2C56-4E4D-9A47-69E3D39ABCF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Milestones - timesStandard-prod" sheetId="1" r:id="rId1"/>
@@ -840,10 +840,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="15" applyFont="1"/>
+    <xf numFmtId="18" fontId="8" fillId="8" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1221,8 +1223,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE01301-CCBB-D24B-BAE4-C62E80B9DF52}">
   <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2920,570 +2922,570 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="1" t="d">
+      <c r="C18" s="4" t="d">
         <v>10:09:59.99999999999946525</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="3">
         <v>1</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="3">
         <v>34</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="3">
         <v>38</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="3">
         <v>44</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="3">
         <v>44</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="3">
         <v>47</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="3">
         <v>48</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="3">
         <v>60</v>
       </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
-      <c r="T18" t="s">
-        <v>40</v>
-      </c>
-      <c r="U18" t="s">
-        <v>40</v>
-      </c>
-      <c r="V18" t="s">
-        <v>40</v>
-      </c>
-      <c r="W18" t="s">
-        <v>40</v>
-      </c>
-      <c r="X18" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y18" t="s">
+      <c r="O18" s="3">
+        <v>0</v>
+      </c>
+      <c r="P18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>0</v>
+      </c>
+      <c r="R18" s="3">
+        <v>0</v>
+      </c>
+      <c r="S18" s="3">
+        <v>0</v>
+      </c>
+      <c r="T18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="W18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="X18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y18" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="Z18" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB18" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE18" t="s">
+      <c r="Z18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AF18">
+      <c r="AF18" s="3">
         <v>5194</v>
       </c>
-      <c r="AI18">
+      <c r="AI18" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="1" t="d">
+      <c r="C19" s="4" t="d">
         <v>09:36:00.00000000000191700</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="3">
         <v>5</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="3">
         <v>11</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="3">
         <v>48</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="3">
         <v>48</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="3">
         <v>49</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="3">
         <v>50</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="3">
         <v>60</v>
       </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19">
-        <v>0</v>
-      </c>
-      <c r="S19">
-        <v>0</v>
-      </c>
-      <c r="T19" t="s">
-        <v>37</v>
-      </c>
-      <c r="U19" t="s">
-        <v>40</v>
-      </c>
-      <c r="V19" t="s">
-        <v>40</v>
-      </c>
-      <c r="W19" t="s">
-        <v>40</v>
-      </c>
-      <c r="X19" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y19" t="s">
+      <c r="O19" s="3">
+        <v>0</v>
+      </c>
+      <c r="P19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>0</v>
+      </c>
+      <c r="R19" s="3">
+        <v>0</v>
+      </c>
+      <c r="S19" s="3">
+        <v>0</v>
+      </c>
+      <c r="T19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="W19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="X19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y19" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="Z19" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB19" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC19" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD19" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE19" t="s">
+      <c r="Z19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AF19">
+      <c r="AF19" s="3">
         <v>5069</v>
       </c>
-      <c r="AI19">
+      <c r="AI19" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="1" t="d">
+      <c r="C20" s="4" t="d">
         <v>19:13:00.00000000000362550</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="3">
         <v>13</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="3">
         <v>51</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="3">
         <v>57</v>
       </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-      <c r="T20" t="s">
-        <v>40</v>
-      </c>
-      <c r="U20" t="s">
-        <v>40</v>
-      </c>
-      <c r="V20" t="s">
-        <v>40</v>
-      </c>
-      <c r="W20" t="s">
-        <v>40</v>
-      </c>
-      <c r="X20" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y20" t="s">
+      <c r="O20" s="3">
+        <v>0</v>
+      </c>
+      <c r="P20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>0</v>
+      </c>
+      <c r="R20" s="3">
+        <v>0</v>
+      </c>
+      <c r="S20" s="3">
+        <v>0</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="W20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="X20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y20" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="Z20" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB20" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC20" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD20" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE20" t="s">
+      <c r="Z20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AF20">
+      <c r="AF20" s="3">
         <v>5194</v>
       </c>
-      <c r="AH20">
+      <c r="AH20" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="1" t="d">
+      <c r="C21" s="4" t="d">
         <v>17:05:00.00000000000213225</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="3">
         <v>5</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="3">
         <v>10</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="3">
         <v>16</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="3">
         <v>15</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="3">
         <v>19</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="3">
         <v>20</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="3">
         <v>20</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="3">
         <v>28</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="3">
         <v>30</v>
       </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
-      <c r="T21" t="s">
-        <v>40</v>
-      </c>
-      <c r="U21" t="s">
-        <v>40</v>
-      </c>
-      <c r="V21" t="s">
-        <v>40</v>
-      </c>
-      <c r="W21" t="s">
-        <v>40</v>
-      </c>
-      <c r="X21" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y21" t="s">
+      <c r="O21" s="3">
+        <v>0</v>
+      </c>
+      <c r="P21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>0</v>
+      </c>
+      <c r="R21" s="3">
+        <v>0</v>
+      </c>
+      <c r="S21" s="3">
+        <v>0</v>
+      </c>
+      <c r="T21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="U21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="W21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="X21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y21" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="Z21" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA21" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB21" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC21" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD21" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE21" t="s">
+      <c r="Z21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AF21">
+      <c r="AF21" s="3">
         <v>5679</v>
       </c>
-      <c r="AH21">
+      <c r="AH21" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="1" t="d">
+      <c r="C22" s="4" t="d">
         <v>17:13:00.00000000000042375</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="3">
         <v>4</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="3">
         <v>9</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="3">
         <v>18</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="3">
         <v>18</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="3">
         <v>18</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="3">
         <v>18</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="3">
         <v>18</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="3">
         <v>23</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="3">
         <v>32</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="3">
         <v>32</v>
       </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22">
-        <v>0</v>
-      </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-      <c r="R22">
-        <v>0</v>
-      </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
-      <c r="T22" t="s">
-        <v>37</v>
-      </c>
-      <c r="U22" t="s">
-        <v>37</v>
-      </c>
-      <c r="V22" t="s">
-        <v>37</v>
-      </c>
-      <c r="W22" t="s">
-        <v>37</v>
-      </c>
-      <c r="X22" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y22" t="s">
+      <c r="O22" s="3">
+        <v>0</v>
+      </c>
+      <c r="P22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>0</v>
+      </c>
+      <c r="R22" s="3">
+        <v>0</v>
+      </c>
+      <c r="S22" s="3">
+        <v>0</v>
+      </c>
+      <c r="T22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y22" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="Z22" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA22" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC22" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD22" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE22" t="s">
+      <c r="Z22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE22" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AF22">
+      <c r="AF22" s="3">
         <v>5485</v>
       </c>
-      <c r="AI22">
+      <c r="AI22" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C23" s="1" t="d">
+      <c r="C23" s="4" t="d">
         <v>15:09:59.99999999999786775</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="3">
         <v>7</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="3">
         <v>13</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="3">
         <v>23</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="3">
         <v>24</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="3">
         <v>24</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="3">
         <v>24</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="3">
         <v>24</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="3">
         <v>25</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="3">
         <v>27</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="3">
         <v>29</v>
       </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23">
-        <v>0</v>
-      </c>
-      <c r="Q23">
-        <v>0</v>
-      </c>
-      <c r="R23">
-        <v>0</v>
-      </c>
-      <c r="S23">
-        <v>0</v>
-      </c>
-      <c r="T23" t="s">
-        <v>37</v>
-      </c>
-      <c r="U23" t="s">
-        <v>37</v>
-      </c>
-      <c r="V23" t="s">
-        <v>37</v>
-      </c>
-      <c r="W23" t="s">
-        <v>37</v>
-      </c>
-      <c r="X23" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y23" t="s">
+      <c r="O23" s="3">
+        <v>0</v>
+      </c>
+      <c r="P23" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>0</v>
+      </c>
+      <c r="R23" s="3">
+        <v>0</v>
+      </c>
+      <c r="S23" s="3">
+        <v>0</v>
+      </c>
+      <c r="T23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y23" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="Z23" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC23" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD23" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE23" t="s">
+      <c r="Z23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE23" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AF23">
+      <c r="AF23" s="3">
         <v>5485</v>
       </c>
-      <c r="AG23">
+      <c r="AG23" s="3">
         <v>11</v>
       </c>
     </row>
@@ -3671,7 +3673,7 @@
         <v>37</v>
       </c>
       <c r="AB25" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="AC25" t="s">
         <v>37</v>
@@ -3772,7 +3774,7 @@
         <v>37</v>
       </c>
       <c r="AB26" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="AC26" t="s">
         <v>37</v>
@@ -3873,7 +3875,7 @@
         <v>37</v>
       </c>
       <c r="AB27" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="AC27" t="s">
         <v>37</v>
@@ -3974,7 +3976,7 @@
         <v>37</v>
       </c>
       <c r="AB28" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="AC28" t="s">
         <v>37</v>
@@ -3998,7 +4000,7 @@
         <v>7.333333333333333</v>
       </c>
       <c r="F29">
-        <f t="shared" ref="F29:N29" si="0">AVERAGE(F2:F28)</f>
+        <f t="shared" ref="F29:M29" si="0">AVERAGE(F2:F28)</f>
         <v>19.37037037037037</v>
       </c>
       <c r="G29">
@@ -4049,7 +4051,7 @@
         <v>9.75</v>
       </c>
       <c r="F30">
-        <f t="shared" ref="F30:N30" si="1">AVERAGE(F2,F6,F9,F12,F13,F16,F17,F20,F21,F23,F25,F26)</f>
+        <f t="shared" ref="F30:M30" si="1">AVERAGE(F2,F6,F9,F12,F13,F16,F17,F20,F21,F23,F25,F26)</f>
         <v>20.916666666666668</v>
       </c>
       <c r="G30">
@@ -4100,7 +4102,7 @@
         <v>5.3571428571428568</v>
       </c>
       <c r="F31">
-        <f t="shared" ref="F31:N31" si="2">AVERAGE(F3,F4,F5,F7,F10,F11,F14,F15,F18,F19,F22,F24,F27,F28)</f>
+        <f t="shared" ref="F31:M31" si="2">AVERAGE(F3,F4,F5,F7,F10,F11,F14,F15,F18,F19,F22,F24,F27,F28)</f>
         <v>18.571428571428573</v>
       </c>
       <c r="G31">

</xml_diff>